<commit_message>
Update time management plot
</commit_message>
<xml_diff>
--- a/misc/time.xlsx
+++ b/misc/time.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pawel\Desktop\GitHub\Inanis\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A72156-7E3D-4678-9C4A-52135911F692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B992D-9A1F-4686-BFE6-25A90E38B5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D79C9EA-BB85-4D32-B74A-64ADD671A99E}"/>
+    <workbookView xWindow="3315" yWindow="2505" windowWidth="21600" windowHeight="11715" xr2:uid="{5D79C9EA-BB85-4D32-B74A-64ADD671A99E}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,9 +37,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Move number</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>Allocated time</t>
@@ -74,6 +70,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>Remaining time</t>
   </si>
 </sst>
 </file>
@@ -206,354 +205,15 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Old time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$B$2:$B$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>280.33333333333331</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>270.98888888888888</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>261.9559259259259</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>253.22406172839504</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>244.78325967078189</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>236.62381768175584</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>228.73635709236399</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>221.11181185595186</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>213.74141812742013</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>206.61670418983945</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>199.72948071684482</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>193.07183135961665</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>186.63610364762943</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>180.41490019270844</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>174.40107018628484</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>168.58770118007536</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>162.96811114073952</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>157.53584076938154</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>152.28464607706883</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>147.20849120783319</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>142.30154150090542</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>137.55815678420856</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>132.97288489140161</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>128.54045539502155</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>124.25577354852084</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>120.1139144302368</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>116.11011728256224</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>112.23978003981017</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>108.49845403848316</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>104.88183890386705</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>101.38577760707147</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>98.006251686835753</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>94.739376630607893</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>91.581397409587623</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>88.528684162601365</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>85.577728023847982</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>82.725137089719709</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>79.967632520062381</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>77.302044769393632</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>74.725309943747177</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>72.234466278955608</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>69.826650736323757</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>67.499095711779631</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>65.249125854720305</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>63.074154992896297</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>60.971683159799753</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>58.939293721139762</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>56.974650597101771</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>55.075495577198382</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>53.239645724625099</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>51.464990867137594</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>49.749491171566341</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>48.091174799180799</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>46.488135639208103</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>44.938531117901164</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>43.440580080637794</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>41.992560744616533</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>40.592808719795983</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>39.239715095802786</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>37.931724592609363</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>36.66733377285572</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>35.445089313760526</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>34.263586336635178</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>33.121466792080675</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>32.017417899011321</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>30.950170635710943</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>29.918498281187244</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>28.921215005147669</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>27.957174504976081</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>27.025268688143544</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>26.124426398538759</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>25.253612185254134</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>24.41182511241233</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>23.598097608665253</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>22.811494355043077</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>22.051111209874975</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>21.316074169545811</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>20.605538363894283</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>19.918687085097808</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>19.254730848927881</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>18.612906487296954</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>17.992476271053722</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>17.392727062018597</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>16.812969493284644</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>16.252537176841823</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>15.710785937613762</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>15.187093073026636</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>14.680856637259081</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>14.191494749350445</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>13.718444924372097</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>13.261163426893027</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>12.819124645996594</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>12.391820491130041</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>11.978759808092372</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>11.579467814489293</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>11.193485554006317</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>10.820369368872774</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>10.459690389910348</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1DEF-4AB1-BBA2-CCDD82CD2426}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Arkusz1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time</c:v>
+                  <c:v>Remaining time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -578,301 +238,301 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>294.9252370559127</c:v>
+                  <c:v>294.60407709351909</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>289.8147813272729</c:v>
+                  <c:v>289.13870082346085</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>284.66231675598215</c:v>
+                  <c:v>283.59555176507223</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>279.46162374532952</c:v>
+                  <c:v>277.96625305200899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>274.20659703496329</c:v>
+                  <c:v>272.24239468184697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>268.89127285670656</c:v>
+                  <c:v>266.4155731669394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>263.50986696402208</c:v>
+                  <c:v>260.47745023795574</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>258.05682538515327</c:v>
+                  <c:v>254.41983511614282</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>252.52689000767688</c:v>
+                  <c:v>248.23479577586912</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>246.91518134083961</c:v>
+                  <c:v>241.91480559224593</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>241.21730099121589</c:v>
+                  <c:v>235.45293274821779</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>235.42945648195962</c:v>
+                  <c:v>228.8430806503838</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>229.54861098241392</c:v>
+                  <c:v>222.08028818840842</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>223.57266020602975</c:v>
+                  <c:v>215.16109868110937</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>217.50063806651997</c:v>
+                  <c:v>208.08400535695472</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>211.33295151308795</c:v>
+                  <c:v>200.84997862059305</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>205.07164312974717</c:v>
+                  <c:v>193.4630753749598</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>198.72067740511878</c:v>
+                  <c:v>185.93112235204839</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>192.2862428993042</c:v>
+                  <c:v>178.26645275298162</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>185.77705776172593</c:v>
+                  <c:v>170.48665771062451</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>179.20466023770734</c:v>
+                  <c:v>162.61529103978586</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>172.58365923335677</c:v>
+                  <c:v>154.68243870552521</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>165.93191333719145</c:v>
+                  <c:v>146.72503702271587</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>159.27060103235712</c:v>
+                  <c:v>138.78680259755168</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>152.62414178039856</c:v>
+                  <c:v>130.91763264037203</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>146.01992920810818</c:v>
+                  <c:v>123.17235879258892</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>139.48784582550175</c:v>
+                  <c:v>115.6088015688476</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>133.0595450312918</c:v>
+                  <c:v>108.28517843576937</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>126.76751073313326</c:v>
+                  <c:v>101.25705394358526</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>120.64393565624751</c:v>
+                  <c:v>94.685081757664733</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>114.71949169751979</c:v>
+                  <c:v>88.539655839193145</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>109.02209274855304</c:v>
+                  <c:v>82.79309169512527</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>103.57576492099284</c:v>
+                  <c:v>77.419501662475483</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>98.399735478957155</c:v>
+                  <c:v>72.394678287137197</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>93.507828509357836</c:v>
+                  <c:v>67.695985271865325</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>88.859120911004112</c:v>
+                  <c:v>63.302255502154111</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>84.441522115832882</c:v>
+                  <c:v>59.19369569062755</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>80.243542633963699</c:v>
+                  <c:v>55.351797210375615</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>76.25426417131608</c:v>
+                  <c:v>51.759252715549856</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>72.463311232818597</c:v>
+                  <c:v>48.399878173602943</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>68.86082413735403</c:v>
+                  <c:v>45.258539957935731</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>65.437433374256784</c:v>
+                  <c:v>42.321086672511861</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>62.18423523466754</c:v>
+                  <c:v>39.574285401317063</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>59.092768654366353</c:v>
+                  <c:v>37.005762095473706</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>56.154993207855789</c:v>
+                  <c:v>34.603945829460841</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>53.363268196460226</c:v>
+                  <c:v>32.358016675319924</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>50.710332776052653</c:v>
+                  <c:v>30.257856960025073</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.189287072724291</c:v>
+                  <c:v>28.294005686437387</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>45.793574237281817</c:v>
+                  <c:v>26.45761591251464</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>43.516963391898713</c:v>
+                  <c:v>24.740414896774144</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41.35353342456763</c:v>
+                  <c:v>23.134666830468348</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>39.297657589205635</c:v>
+                  <c:v>21.633137988585542</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>37.343988871359606</c:v>
+                  <c:v>20.229064142684638</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>35.487446081450273</c:v>
+                  <c:v>18.91612008876228</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>33.723200639385531</c:v>
+                  <c:v>17.688391152878559</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>32.046664016171896</c:v>
+                  <c:v>16.540346546177208</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>30.453475799861661</c:v>
+                  <c:v>15.466814449267432</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>28.93949235479716</c:v>
+                  <c:v>14.462958713725179</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>27.50077604465654</c:v>
+                  <c:v>13.524257075756573</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>26.133584991271903</c:v>
+                  <c:v>12.646480783878372</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>24.834363342584052</c:v>
+                  <c:v>11.825675548840302</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>23.599732024422341</c:v>
+                  <c:v>11.058143729970684</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>22.42647995205639</c:v>
+                  <c:v>10.340427677696749</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>21.31155567866233</c:v>
+                  <c:v>9.669294157199424</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>20.252059458982483</c:v>
+                  <c:v>9.0417197830328302</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>19.245235707537311</c:v>
+                  <c:v>8.4548773990929842</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>18.288465831774623</c:v>
+                  <c:v>7.9061233425789066</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>17.379261421516127</c:v>
+                  <c:v>7.3929855345716327</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>16.515257776988197</c:v>
+                  <c:v>6.9131523435804425</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>15.694207758604204</c:v>
+                  <c:v>6.4644621718877646</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>14.913975942502688</c:v>
+                  <c:v>6.0448937177803437</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>14.172533066640817</c:v>
+                  <c:v>5.6525568697990485</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>13.467950752998282</c:v>
+                  <c:v>5.2856841919868893</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>12.798396492164908</c:v>
+                  <c:v>4.9426229617771753</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>12.162128877267653</c:v>
+                  <c:v>4.6218277246533566</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>11.557493074841194</c:v>
+                  <c:v>4.3218533320400656</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>10.982916520862528</c:v>
+                  <c:v>4.0413484310618095</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>10.436904830755653</c:v>
+                  <c:v>3.7790493768413564</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>9.9180379127288578</c:v>
+                  <c:v>3.5337745399133649</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>9.4249662743360485</c:v>
+                  <c:v>3.3044189831087616</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>8.9564075126560159</c:v>
+                  <c:v>3.0899494839297925</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>8.5111429789611748</c:v>
+                  <c:v>2.8893998799920753</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>8.088014609201073</c:v>
+                  <c:v>2.7018667165653607</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>7.6859219120572586</c:v>
+                  <c:v>2.5265051766056366</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>7.3038191067359017</c:v>
+                  <c:v>2.362525274943799</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>6.9407124030540128</c:v>
+                  <c:v>2.2091882994861152</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>6.5956574167451798</c:v>
+                  <c:v>2.0658034833944594</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6.2677567132624441</c:v>
+                  <c:v>1.9317248932548514</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>5.9561574736901148</c:v>
+                  <c:v>1.8063485192158213</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>5.6600492766939281</c:v>
+                  <c:v>1.6891095539879852</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>5.3786619907407482</c:v>
+                  <c:v>1.5794798484470123</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>5.1112637711057944</c:v>
+                  <c:v>1.4769655323777431</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.8571591564579233</c:v>
+                  <c:v>1.381104789641165</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.6156872600724812</c:v>
+                  <c:v>1.2914657777416056</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>4.386220050967351</c:v>
+                  <c:v>1.2076446824220164</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>4.1681607204916915</c:v>
+                  <c:v>1.1292638985235024</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>3.9609421301191201</c:v>
+                  <c:v>1.0559703289140658</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.7640253364082978</c:v>
+                  <c:v>0.98743379382341356</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>3.5768981892945555</c:v>
+                  <c:v>0.9233455434180543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1256,350 +916,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Old allocated time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$C$2:$C$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.6666666666666661</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.3444444444444432</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.0329629629629622</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.7318641975308626</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.4408020576131673</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.1594419890260621</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.8874605893918615</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.6245452364121329</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.3703937285317283</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.1247139375806707</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.8872234729946484</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.657649357228161</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.435727711987222</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.2212034549209809</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.013830006423615</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.8133690062094949</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.6195900393358453</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.4322703713579843</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.2511946923127182</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.0761548692356273</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.9069497069277732</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.7433847166968475</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.5852718928069525</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4.4324294963800535</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4.2846818465007184</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4.1418591182840281</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.0037971476745602</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.8703372427520746</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.7413260013270055</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.6166151346161053</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.4960612967955682</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.3795259202357157</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.2668750562278586</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.1579792210202631</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.0527132469862539</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2.9509561387533787</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2.852590934128266</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2.7575045696573235</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2.6655877506687462</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.5767348256464544</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.4908436647915724</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2.4078155426318535</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2.3275550245441252</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2.249969857059321</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2.17497086182401</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2.1024718330965433</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2.0323894386599917</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.964643124037992</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.8991550199033924</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1.8358498525732794</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1.7746548574875034</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.7154996955712531</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.6583163723855447</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1.6030391599726932</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1.5496045213069367</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1.4979510372633722</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1.4480193360212599</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1.3997520248205511</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1.3530936239931994</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.3079905031934262</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1.2643908197536455</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1.2222444590951906</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1.1815029771253509</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1.142119544554506</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1.1040488930693557</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1.0672472633003773</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1.0316723545236981</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.99728327603957478</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.96404050017158893</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.93190581683253604</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.90084228960478485</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.87081421328462527</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.84178707284180443</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.8137275037470777</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.78660325362217509</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.76038314516810257</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.73503704032916584</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.71053580565152707</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.68685127879647612</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.66395623616992694</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.64182436163092937</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.6204302162432318</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.59974920903512408</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.57975756873395323</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.56043231644282143</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.54175123922806079</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.52369286458712538</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.5062364357675545</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.48936188790863605</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.47304982497834819</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.45728149747906988</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.44203878089643422</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.4273041548665531</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.41306068303766802</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.39929199360307904</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.38598226048297646</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.37311618513354389</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.36067897896242579</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.34865634633034492</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1DEF-4AB1-BBA2-CCDD82CD2426}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Arkusz1!$E$1</c:f>
@@ -1630,304 +948,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>5.0747629440872721</c:v>
+                  <c:v>5.3959229064809149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1104557286397991</c:v>
+                  <c:v>5.4653762700582309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.152464571290742</c:v>
+                  <c:v>5.5431490583886323</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.200693010652639</c:v>
+                  <c:v>5.6292987130632115</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2550267103662334</c:v>
+                  <c:v>5.7238583701620156</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3153241782567546</c:v>
+                  <c:v>5.8268215149075884</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3814058926844668</c:v>
+                  <c:v>5.938122928983681</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4530415788688078</c:v>
+                  <c:v>6.0576151218129244</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.5299353774763791</c:v>
+                  <c:v>6.1850393402737032</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.6117086668372638</c:v>
+                  <c:v>6.3199901836231778</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.6978803496237074</c:v>
+                  <c:v>6.4618728440281314</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.7878445092562716</c:v>
+                  <c:v>6.6098520978339792</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.8808454995457096</c:v>
+                  <c:v>6.7627924619753772</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9759507763841633</c:v>
+                  <c:v>6.9191895072990448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.0720221395097882</c:v>
+                  <c:v>7.0770933241546441</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.1676865534320298</c:v>
+                  <c:v>7.2340267363616562</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.2613083833407872</c:v>
+                  <c:v>7.3869032456332553</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.350965724628403</c:v>
+                  <c:v>7.531953022911404</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.4344345058145915</c:v>
+                  <c:v>7.6646695990667615</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.5091851375782834</c:v>
+                  <c:v>7.7797950423571027</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.5723975240185704</c:v>
+                  <c:v>7.8713666708386656</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.6210010043505765</c:v>
+                  <c:v>7.9328523342606472</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.6517458961653304</c:v>
+                  <c:v>7.9574016828093432</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.6613123048343255</c:v>
+                  <c:v>7.9382344251641843</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.6464592519585617</c:v>
+                  <c:v>7.8691699571796541</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.6042125722903666</c:v>
+                  <c:v>7.7452738477831105</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.5320833826064275</c:v>
+                  <c:v>7.5635572237413333</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.4283007942099459</c:v>
+                  <c:v>7.3236231330782235</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.2920342981585389</c:v>
+                  <c:v>7.0281244921841006</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.1235750768857535</c:v>
+                  <c:v>6.5719721859205338</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.9244439587277204</c:v>
+                  <c:v>6.1454259184715854</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.6973989489667547</c:v>
+                  <c:v>5.746564144067877</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.4463278275601921</c:v>
+                  <c:v>5.3735900326497879</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.1760294420356869</c:v>
+                  <c:v>5.0248233753382898</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.8919069695993134</c:v>
+                  <c:v>4.6986930152718687</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.6487075983537274</c:v>
+                  <c:v>4.3937297697112161</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.4175987951712319</c:v>
+                  <c:v>4.1085598115265647</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.1979794818691847</c:v>
+                  <c:v>3.8418984802519351</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.9892784626476199</c:v>
+                  <c:v>3.592544494825761</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.7909529384974898</c:v>
+                  <c:v>3.3593745419469121</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.6024870954645611</c:v>
+                  <c:v>3.1413382156672132</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.4233907630972511</c:v>
+                  <c:v>2.9374532854238717</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.2531981395892471</c:v>
+                  <c:v>2.7468012711947973</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.0914665803011898</c:v>
+                  <c:v>2.5685233058433572</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.9377754465105625</c:v>
+                  <c:v>2.4018162660128688</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.7917250113955605</c:v>
+                  <c:v>2.2459291541409154</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.6529354204075726</c:v>
+                  <c:v>2.1001597152948506</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.5210457033283635</c:v>
+                  <c:v>1.9638512735876847</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.3957128354424757</c:v>
+                  <c:v>1.8363897739227468</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.2766108453831042</c:v>
+                  <c:v>1.7172010157404953</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.1634299673310831</c:v>
+                  <c:v>1.6057480663057959</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.0558758353619968</c:v>
+                  <c:v>1.5015288418828054</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.9536687178460264</c:v>
+                  <c:v>1.4040738459009041</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.8565427899093305</c:v>
+                  <c:v>1.3129440539223594</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.7642454420647418</c:v>
+                  <c:v>1.22772893588372</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.6765366232136385</c:v>
+                  <c:v>1.1480446067013501</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.5931882163102362</c:v>
+                  <c:v>1.0735320969097759</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.5139834450645022</c:v>
+                  <c:v>1.003855735542253</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.4387163101406197</c:v>
+                  <c:v>0.93870163796860517</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.3671910533846379</c:v>
+                  <c:v>0.87777629187820028</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.2992216486878498</c:v>
+                  <c:v>0.82080523503807135</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.2346313181617117</c:v>
+                  <c:v>0.76753181886961785</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.1732520723659499</c:v>
+                  <c:v>0.71771605227393487</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.114924273394059</c:v>
+                  <c:v>0.67113352049732466</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.0594962196798474</c:v>
+                  <c:v>0.62757437416659378</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.0068237514451708</c:v>
+                  <c:v>0.58684238393984645</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.95676987576268946</c:v>
+                  <c:v>0.54875405651407805</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.9092044102584953</c:v>
+                  <c:v>0.51313780800727415</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.86400364452792966</c:v>
+                  <c:v>0.47983319099119043</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.82105001838399294</c:v>
+                  <c:v>0.44869017169267794</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.78023181610151604</c:v>
+                  <c:v>0.41956845410742127</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.74144287586187108</c:v>
+                  <c:v>0.39233684798129492</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.70458231364253365</c:v>
+                  <c:v>0.36687267781215921</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.66955426083337333</c:v>
+                  <c:v>0.34306123020971357</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.63626761489725547</c:v>
+                  <c:v>0.32079523712381902</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.60463580242646042</c:v>
+                  <c:v>0.29997439261329117</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.57457655397866547</c:v>
+                  <c:v>0.28050490097825581</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.54601169010687511</c:v>
+                  <c:v>0.26229905422045297</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.51886691802679441</c:v>
+                  <c:v>0.24527483692799157</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.49307163839281004</c:v>
+                  <c:v>0.22935555680460346</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.46855876168003313</c:v>
+                  <c:v>0.21446949917896915</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.44526453369484154</c:v>
+                  <c:v>0.20054960393771734</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.42312836976010221</c:v>
+                  <c:v>0.18753316342671475</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.40209269714381468</c:v>
+                  <c:v>0.17536153995972434</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.38210280532135693</c:v>
+                  <c:v>0.16397990166183754</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.3631067036818893</c:v>
+                  <c:v>0.15333697545768391</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.34505498630883269</c:v>
+                  <c:v>0.14338481609165568</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.32790070348273559</c:v>
+                  <c:v>0.13407859013960793</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.3115992395723296</c:v>
+                  <c:v>0.12537637403903013</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.29610819699618673</c:v>
+                  <c:v>0.11723896522783614</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.28138728595317991</c:v>
+                  <c:v>0.10962970554097307</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.26739821963495419</c:v>
+                  <c:v>0.10251431606926924</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.25410461464787154</c:v>
+                  <c:v>9.5860742736578131E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.24147189638544192</c:v>
+                  <c:v>8.963901189955939E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.22946720910512988</c:v>
+                  <c:v>8.3821095319589367E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.21805933047565995</c:v>
+                  <c:v>7.8380783898513967E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.20721859037257137</c:v>
+                  <c:v>7.3293569609436629E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.19691679371082216</c:v>
+                  <c:v>6.8536535090652245E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.18712714711374237</c:v>
+                  <c:v>6.4088250405359287E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.17782418922761359</c:v>
+                  <c:v>5.9928676502063689E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2786,9 +2104,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2826,7 +2144,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2932,7 +2250,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3074,7 +2392,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3085,14 +2403,14 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3101,19 +2419,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3132,13 +2450,13 @@
       </c>
       <c r="E2">
         <f>D2 / ($H$3+$H$4*SIN(MIN($H$5,A2+$H$6)/$H$7))</f>
-        <v>5.0747629440872721</v>
+        <v>5.3959229064809149</v>
       </c>
       <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3155,17 +2473,17 @@
       </c>
       <c r="D3">
         <f>D2-E2</f>
-        <v>294.9252370559127</v>
+        <v>294.60407709351909</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" si="1">D3 / ($H$3+$H$4*SIN(MIN($H$5,A3+$H$6)/$H$7))</f>
-        <v>5.1104557286397991</v>
+        <v>5.4653762700582309</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3182,17 +2500,17 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D67" si="3">D3-E3</f>
-        <v>289.8147813272729</v>
+        <v>289.13870082346085</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>5.152464571290742</v>
+        <v>5.5431490583886323</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4">
-        <v>-25</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3209,17 +2527,17 @@
       </c>
       <c r="D5">
         <f t="shared" si="3"/>
-        <v>284.66231675598215</v>
+        <v>283.59555176507223</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>5.200693010652639</v>
+        <v>5.6292987130632115</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3236,17 +2554,17 @@
       </c>
       <c r="D6">
         <f t="shared" si="3"/>
-        <v>279.46162374532952</v>
+        <v>277.96625305200899</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>5.2550267103662334</v>
+        <v>5.7238583701620156</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>-10</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3263,14 +2581,14 @@
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
-        <v>274.20659703496329</v>
+        <v>272.24239468184697</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>5.3153241782567546</v>
+        <v>5.8268215149075884</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>15</v>
@@ -3290,11 +2608,11 @@
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
-        <v>268.89127285670656</v>
+        <v>266.4155731669394</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>5.3814058926844668</v>
+        <v>5.938122928983681</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3311,11 +2629,11 @@
       </c>
       <c r="D9">
         <f t="shared" si="3"/>
-        <v>263.50986696402208</v>
+        <v>260.47745023795574</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>5.4530415788688078</v>
+        <v>6.0576151218129244</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3332,11 +2650,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
-        <v>258.05682538515327</v>
+        <v>254.41983511614282</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>5.5299353774763791</v>
+        <v>6.1850393402737032</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3353,11 +2671,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
-        <v>252.52689000767688</v>
+        <v>248.23479577586912</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>5.6117086668372638</v>
+        <v>6.3199901836231778</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3374,11 +2692,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>246.91518134083961</v>
+        <v>241.91480559224593</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>5.6978803496237074</v>
+        <v>6.4618728440281314</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3395,11 +2713,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
-        <v>241.21730099121589</v>
+        <v>235.45293274821779</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>5.7878445092562716</v>
+        <v>6.6098520978339792</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3416,11 +2734,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
-        <v>235.42945648195962</v>
+        <v>228.8430806503838</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>5.8808454995457096</v>
+        <v>6.7627924619753772</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3437,11 +2755,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="3"/>
-        <v>229.54861098241392</v>
+        <v>222.08028818840842</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>5.9759507763841633</v>
+        <v>6.9191895072990448</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3458,11 +2776,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="3"/>
-        <v>223.57266020602975</v>
+        <v>215.16109868110937</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>6.0720221395097882</v>
+        <v>7.0770933241546441</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3479,11 +2797,11 @@
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>217.50063806651997</v>
+        <v>208.08400535695472</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>6.1676865534320298</v>
+        <v>7.2340267363616562</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3500,11 +2818,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
-        <v>211.33295151308795</v>
+        <v>200.84997862059305</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>6.2613083833407872</v>
+        <v>7.3869032456332553</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3521,11 +2839,11 @@
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>205.07164312974717</v>
+        <v>193.4630753749598</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>6.350965724628403</v>
+        <v>7.531953022911404</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3542,11 +2860,11 @@
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>198.72067740511878</v>
+        <v>185.93112235204839</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>6.4344345058145915</v>
+        <v>7.6646695990667615</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3563,11 +2881,11 @@
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>192.2862428993042</v>
+        <v>178.26645275298162</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>6.5091851375782834</v>
+        <v>7.7797950423571027</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3584,11 +2902,11 @@
       </c>
       <c r="D22">
         <f t="shared" si="3"/>
-        <v>185.77705776172593</v>
+        <v>170.48665771062451</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>6.5723975240185704</v>
+        <v>7.8713666708386656</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3605,11 +2923,11 @@
       </c>
       <c r="D23">
         <f t="shared" si="3"/>
-        <v>179.20466023770734</v>
+        <v>162.61529103978586</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>6.6210010043505765</v>
+        <v>7.9328523342606472</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3626,11 +2944,11 @@
       </c>
       <c r="D24">
         <f t="shared" si="3"/>
-        <v>172.58365923335677</v>
+        <v>154.68243870552521</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>6.6517458961653304</v>
+        <v>7.9574016828093432</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3647,11 +2965,11 @@
       </c>
       <c r="D25">
         <f t="shared" si="3"/>
-        <v>165.93191333719145</v>
+        <v>146.72503702271587</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>6.6613123048343255</v>
+        <v>7.9382344251641843</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3668,11 +2986,11 @@
       </c>
       <c r="D26">
         <f t="shared" si="3"/>
-        <v>159.27060103235712</v>
+        <v>138.78680259755168</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>6.6464592519585617</v>
+        <v>7.8691699571796541</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3689,11 +3007,11 @@
       </c>
       <c r="D27">
         <f t="shared" si="3"/>
-        <v>152.62414178039856</v>
+        <v>130.91763264037203</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>6.6042125722903666</v>
+        <v>7.7452738477831105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3710,11 +3028,11 @@
       </c>
       <c r="D28">
         <f t="shared" si="3"/>
-        <v>146.01992920810818</v>
+        <v>123.17235879258892</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>6.5320833826064275</v>
+        <v>7.5635572237413333</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3731,11 +3049,11 @@
       </c>
       <c r="D29">
         <f t="shared" si="3"/>
-        <v>139.48784582550175</v>
+        <v>115.6088015688476</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>6.4283007942099459</v>
+        <v>7.3236231330782235</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3752,11 +3070,11 @@
       </c>
       <c r="D30">
         <f t="shared" si="3"/>
-        <v>133.0595450312918</v>
+        <v>108.28517843576937</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>6.2920342981585389</v>
+        <v>7.0281244921841006</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3773,11 +3091,11 @@
       </c>
       <c r="D31">
         <f t="shared" si="3"/>
-        <v>126.76751073313326</v>
+        <v>101.25705394358526</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>6.1235750768857535</v>
+        <v>6.5719721859205338</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,11 +3112,11 @@
       </c>
       <c r="D32">
         <f t="shared" si="3"/>
-        <v>120.64393565624751</v>
+        <v>94.685081757664733</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>5.9244439587277204</v>
+        <v>6.1454259184715854</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3815,11 +3133,11 @@
       </c>
       <c r="D33">
         <f t="shared" si="3"/>
-        <v>114.71949169751979</v>
+        <v>88.539655839193145</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>5.6973989489667547</v>
+        <v>5.746564144067877</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3836,11 +3154,11 @@
       </c>
       <c r="D34">
         <f t="shared" si="3"/>
-        <v>109.02209274855304</v>
+        <v>82.79309169512527</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>5.4463278275601921</v>
+        <v>5.3735900326497879</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3857,11 +3175,11 @@
       </c>
       <c r="D35">
         <f t="shared" si="3"/>
-        <v>103.57576492099284</v>
+        <v>77.419501662475483</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>5.1760294420356869</v>
+        <v>5.0248233753382898</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,11 +3196,11 @@
       </c>
       <c r="D36">
         <f t="shared" si="3"/>
-        <v>98.399735478957155</v>
+        <v>72.394678287137197</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>4.8919069695993134</v>
+        <v>4.6986930152718687</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,11 +3217,11 @@
       </c>
       <c r="D37">
         <f t="shared" si="3"/>
-        <v>93.507828509357836</v>
+        <v>67.695985271865325</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>4.6487075983537274</v>
+        <v>4.3937297697112161</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3920,11 +3238,11 @@
       </c>
       <c r="D38">
         <f t="shared" si="3"/>
-        <v>88.859120911004112</v>
+        <v>63.302255502154111</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>4.4175987951712319</v>
+        <v>4.1085598115265647</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3941,11 +3259,11 @@
       </c>
       <c r="D39">
         <f t="shared" si="3"/>
-        <v>84.441522115832882</v>
+        <v>59.19369569062755</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
-        <v>4.1979794818691847</v>
+        <v>3.8418984802519351</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3962,11 +3280,11 @@
       </c>
       <c r="D40">
         <f t="shared" si="3"/>
-        <v>80.243542633963699</v>
+        <v>55.351797210375615</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
-        <v>3.9892784626476199</v>
+        <v>3.592544494825761</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3983,11 +3301,11 @@
       </c>
       <c r="D41">
         <f t="shared" si="3"/>
-        <v>76.25426417131608</v>
+        <v>51.759252715549856</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
-        <v>3.7909529384974898</v>
+        <v>3.3593745419469121</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4004,11 +3322,11 @@
       </c>
       <c r="D42">
         <f t="shared" si="3"/>
-        <v>72.463311232818597</v>
+        <v>48.399878173602943</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
-        <v>3.6024870954645611</v>
+        <v>3.1413382156672132</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -4025,11 +3343,11 @@
       </c>
       <c r="D43">
         <f t="shared" si="3"/>
-        <v>68.86082413735403</v>
+        <v>45.258539957935731</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>3.4233907630972511</v>
+        <v>2.9374532854238717</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -4046,11 +3364,11 @@
       </c>
       <c r="D44">
         <f t="shared" si="3"/>
-        <v>65.437433374256784</v>
+        <v>42.321086672511861</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
-        <v>3.2531981395892471</v>
+        <v>2.7468012711947973</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -4067,11 +3385,11 @@
       </c>
       <c r="D45">
         <f t="shared" si="3"/>
-        <v>62.18423523466754</v>
+        <v>39.574285401317063</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
-        <v>3.0914665803011898</v>
+        <v>2.5685233058433572</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -4088,11 +3406,11 @@
       </c>
       <c r="D46">
         <f t="shared" si="3"/>
-        <v>59.092768654366353</v>
+        <v>37.005762095473706</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
-        <v>2.9377754465105625</v>
+        <v>2.4018162660128688</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -4109,11 +3427,11 @@
       </c>
       <c r="D47">
         <f t="shared" si="3"/>
-        <v>56.154993207855789</v>
+        <v>34.603945829460841</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
-        <v>2.7917250113955605</v>
+        <v>2.2459291541409154</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4130,11 +3448,11 @@
       </c>
       <c r="D48">
         <f t="shared" si="3"/>
-        <v>53.363268196460226</v>
+        <v>32.358016675319924</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
-        <v>2.6529354204075726</v>
+        <v>2.1001597152948506</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -4151,11 +3469,11 @@
       </c>
       <c r="D49">
         <f t="shared" si="3"/>
-        <v>50.710332776052653</v>
+        <v>30.257856960025073</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
-        <v>2.5210457033283635</v>
+        <v>1.9638512735876847</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4172,11 +3490,11 @@
       </c>
       <c r="D50">
         <f t="shared" si="3"/>
-        <v>48.189287072724291</v>
+        <v>28.294005686437387</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
-        <v>2.3957128354424757</v>
+        <v>1.8363897739227468</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4193,11 +3511,11 @@
       </c>
       <c r="D51">
         <f t="shared" si="3"/>
-        <v>45.793574237281817</v>
+        <v>26.45761591251464</v>
       </c>
       <c r="E51">
         <f t="shared" si="1"/>
-        <v>2.2766108453831042</v>
+        <v>1.7172010157404953</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,11 +3532,11 @@
       </c>
       <c r="D52">
         <f t="shared" si="3"/>
-        <v>43.516963391898713</v>
+        <v>24.740414896774144</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
-        <v>2.1634299673310831</v>
+        <v>1.6057480663057959</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -4235,11 +3553,11 @@
       </c>
       <c r="D53">
         <f t="shared" si="3"/>
-        <v>41.35353342456763</v>
+        <v>23.134666830468348</v>
       </c>
       <c r="E53">
         <f t="shared" si="1"/>
-        <v>2.0558758353619968</v>
+        <v>1.5015288418828054</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -4256,11 +3574,11 @@
       </c>
       <c r="D54">
         <f t="shared" si="3"/>
-        <v>39.297657589205635</v>
+        <v>21.633137988585542</v>
       </c>
       <c r="E54">
         <f t="shared" si="1"/>
-        <v>1.9536687178460264</v>
+        <v>1.4040738459009041</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -4277,11 +3595,11 @@
       </c>
       <c r="D55">
         <f t="shared" si="3"/>
-        <v>37.343988871359606</v>
+        <v>20.229064142684638</v>
       </c>
       <c r="E55">
         <f t="shared" si="1"/>
-        <v>1.8565427899093305</v>
+        <v>1.3129440539223594</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -4298,11 +3616,11 @@
       </c>
       <c r="D56">
         <f t="shared" si="3"/>
-        <v>35.487446081450273</v>
+        <v>18.91612008876228</v>
       </c>
       <c r="E56">
         <f t="shared" si="1"/>
-        <v>1.7642454420647418</v>
+        <v>1.22772893588372</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -4319,11 +3637,11 @@
       </c>
       <c r="D57">
         <f t="shared" si="3"/>
-        <v>33.723200639385531</v>
+        <v>17.688391152878559</v>
       </c>
       <c r="E57">
         <f t="shared" si="1"/>
-        <v>1.6765366232136385</v>
+        <v>1.1480446067013501</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -4340,11 +3658,11 @@
       </c>
       <c r="D58">
         <f t="shared" si="3"/>
-        <v>32.046664016171896</v>
+        <v>16.540346546177208</v>
       </c>
       <c r="E58">
         <f t="shared" si="1"/>
-        <v>1.5931882163102362</v>
+        <v>1.0735320969097759</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -4361,11 +3679,11 @@
       </c>
       <c r="D59">
         <f t="shared" si="3"/>
-        <v>30.453475799861661</v>
+        <v>15.466814449267432</v>
       </c>
       <c r="E59">
         <f t="shared" si="1"/>
-        <v>1.5139834450645022</v>
+        <v>1.003855735542253</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -4382,11 +3700,11 @@
       </c>
       <c r="D60">
         <f t="shared" si="3"/>
-        <v>28.93949235479716</v>
+        <v>14.462958713725179</v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
-        <v>1.4387163101406197</v>
+        <v>0.93870163796860517</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4403,11 +3721,11 @@
       </c>
       <c r="D61">
         <f t="shared" si="3"/>
-        <v>27.50077604465654</v>
+        <v>13.524257075756573</v>
       </c>
       <c r="E61">
         <f t="shared" si="1"/>
-        <v>1.3671910533846379</v>
+        <v>0.87777629187820028</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4424,11 +3742,11 @@
       </c>
       <c r="D62">
         <f t="shared" si="3"/>
-        <v>26.133584991271903</v>
+        <v>12.646480783878372</v>
       </c>
       <c r="E62">
         <f t="shared" si="1"/>
-        <v>1.2992216486878498</v>
+        <v>0.82080523503807135</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4445,11 +3763,11 @@
       </c>
       <c r="D63">
         <f t="shared" si="3"/>
-        <v>24.834363342584052</v>
+        <v>11.825675548840302</v>
       </c>
       <c r="E63">
         <f t="shared" si="1"/>
-        <v>1.2346313181617117</v>
+        <v>0.76753181886961785</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4466,11 +3784,11 @@
       </c>
       <c r="D64">
         <f t="shared" si="3"/>
-        <v>23.599732024422341</v>
+        <v>11.058143729970684</v>
       </c>
       <c r="E64">
         <f t="shared" si="1"/>
-        <v>1.1732520723659499</v>
+        <v>0.71771605227393487</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -4487,11 +3805,11 @@
       </c>
       <c r="D65">
         <f t="shared" si="3"/>
-        <v>22.42647995205639</v>
+        <v>10.340427677696749</v>
       </c>
       <c r="E65">
         <f t="shared" si="1"/>
-        <v>1.114924273394059</v>
+        <v>0.67113352049732466</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -4508,11 +3826,11 @@
       </c>
       <c r="D66">
         <f t="shared" si="3"/>
-        <v>21.31155567866233</v>
+        <v>9.669294157199424</v>
       </c>
       <c r="E66">
         <f t="shared" si="1"/>
-        <v>1.0594962196798474</v>
+        <v>0.62757437416659378</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4529,11 +3847,11 @@
       </c>
       <c r="D67">
         <f t="shared" si="3"/>
-        <v>20.252059458982483</v>
+        <v>9.0417197830328302</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E101" si="5">D67 / ($H$3+$H$4*SIN(MIN($H$5,A67+$H$6)/$H$7))</f>
-        <v>1.0068237514451708</v>
+        <v>0.58684238393984645</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4550,11 +3868,11 @@
       </c>
       <c r="D68">
         <f t="shared" ref="D68:D101" si="7">D67-E67</f>
-        <v>19.245235707537311</v>
+        <v>8.4548773990929842</v>
       </c>
       <c r="E68">
         <f t="shared" si="5"/>
-        <v>0.95676987576268946</v>
+        <v>0.54875405651407805</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4571,11 +3889,11 @@
       </c>
       <c r="D69">
         <f t="shared" si="7"/>
-        <v>18.288465831774623</v>
+        <v>7.9061233425789066</v>
       </c>
       <c r="E69">
         <f t="shared" si="5"/>
-        <v>0.9092044102584953</v>
+        <v>0.51313780800727415</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4592,11 +3910,11 @@
       </c>
       <c r="D70">
         <f t="shared" si="7"/>
-        <v>17.379261421516127</v>
+        <v>7.3929855345716327</v>
       </c>
       <c r="E70">
         <f t="shared" si="5"/>
-        <v>0.86400364452792966</v>
+        <v>0.47983319099119043</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4613,11 +3931,11 @@
       </c>
       <c r="D71">
         <f t="shared" si="7"/>
-        <v>16.515257776988197</v>
+        <v>6.9131523435804425</v>
       </c>
       <c r="E71">
         <f t="shared" si="5"/>
-        <v>0.82105001838399294</v>
+        <v>0.44869017169267794</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4634,11 +3952,11 @@
       </c>
       <c r="D72">
         <f t="shared" si="7"/>
-        <v>15.694207758604204</v>
+        <v>6.4644621718877646</v>
       </c>
       <c r="E72">
         <f t="shared" si="5"/>
-        <v>0.78023181610151604</v>
+        <v>0.41956845410742127</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -4655,11 +3973,11 @@
       </c>
       <c r="D73">
         <f t="shared" si="7"/>
-        <v>14.913975942502688</v>
+        <v>6.0448937177803437</v>
       </c>
       <c r="E73">
         <f t="shared" si="5"/>
-        <v>0.74144287586187108</v>
+        <v>0.39233684798129492</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4676,11 +3994,11 @@
       </c>
       <c r="D74">
         <f t="shared" si="7"/>
-        <v>14.172533066640817</v>
+        <v>5.6525568697990485</v>
       </c>
       <c r="E74">
         <f t="shared" si="5"/>
-        <v>0.70458231364253365</v>
+        <v>0.36687267781215921</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4697,11 +4015,11 @@
       </c>
       <c r="D75">
         <f t="shared" si="7"/>
-        <v>13.467950752998282</v>
+        <v>5.2856841919868893</v>
       </c>
       <c r="E75">
         <f t="shared" si="5"/>
-        <v>0.66955426083337333</v>
+        <v>0.34306123020971357</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4718,11 +4036,11 @@
       </c>
       <c r="D76">
         <f t="shared" si="7"/>
-        <v>12.798396492164908</v>
+        <v>4.9426229617771753</v>
       </c>
       <c r="E76">
         <f t="shared" si="5"/>
-        <v>0.63626761489725547</v>
+        <v>0.32079523712381902</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4739,11 +4057,11 @@
       </c>
       <c r="D77">
         <f t="shared" si="7"/>
-        <v>12.162128877267653</v>
+        <v>4.6218277246533566</v>
       </c>
       <c r="E77">
         <f t="shared" si="5"/>
-        <v>0.60463580242646042</v>
+        <v>0.29997439261329117</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -4760,11 +4078,11 @@
       </c>
       <c r="D78">
         <f t="shared" si="7"/>
-        <v>11.557493074841194</v>
+        <v>4.3218533320400656</v>
       </c>
       <c r="E78">
         <f t="shared" si="5"/>
-        <v>0.57457655397866547</v>
+        <v>0.28050490097825581</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -4781,11 +4099,11 @@
       </c>
       <c r="D79">
         <f t="shared" si="7"/>
-        <v>10.982916520862528</v>
+        <v>4.0413484310618095</v>
       </c>
       <c r="E79">
         <f t="shared" si="5"/>
-        <v>0.54601169010687511</v>
+        <v>0.26229905422045297</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4802,11 +4120,11 @@
       </c>
       <c r="D80">
         <f t="shared" si="7"/>
-        <v>10.436904830755653</v>
+        <v>3.7790493768413564</v>
       </c>
       <c r="E80">
         <f t="shared" si="5"/>
-        <v>0.51886691802679441</v>
+        <v>0.24527483692799157</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4823,11 +4141,11 @@
       </c>
       <c r="D81">
         <f t="shared" si="7"/>
-        <v>9.9180379127288578</v>
+        <v>3.5337745399133649</v>
       </c>
       <c r="E81">
         <f t="shared" si="5"/>
-        <v>0.49307163839281004</v>
+        <v>0.22935555680460346</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4844,11 +4162,11 @@
       </c>
       <c r="D82">
         <f t="shared" si="7"/>
-        <v>9.4249662743360485</v>
+        <v>3.3044189831087616</v>
       </c>
       <c r="E82">
         <f t="shared" si="5"/>
-        <v>0.46855876168003313</v>
+        <v>0.21446949917896915</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4865,11 +4183,11 @@
       </c>
       <c r="D83">
         <f t="shared" si="7"/>
-        <v>8.9564075126560159</v>
+        <v>3.0899494839297925</v>
       </c>
       <c r="E83">
         <f t="shared" si="5"/>
-        <v>0.44526453369484154</v>
+        <v>0.20054960393771734</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4886,11 +4204,11 @@
       </c>
       <c r="D84">
         <f t="shared" si="7"/>
-        <v>8.5111429789611748</v>
+        <v>2.8893998799920753</v>
       </c>
       <c r="E84">
         <f t="shared" si="5"/>
-        <v>0.42312836976010221</v>
+        <v>0.18753316342671475</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4907,11 +4225,11 @@
       </c>
       <c r="D85">
         <f t="shared" si="7"/>
-        <v>8.088014609201073</v>
+        <v>2.7018667165653607</v>
       </c>
       <c r="E85">
         <f t="shared" si="5"/>
-        <v>0.40209269714381468</v>
+        <v>0.17536153995972434</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4928,11 +4246,11 @@
       </c>
       <c r="D86">
         <f t="shared" si="7"/>
-        <v>7.6859219120572586</v>
+        <v>2.5265051766056366</v>
       </c>
       <c r="E86">
         <f t="shared" si="5"/>
-        <v>0.38210280532135693</v>
+        <v>0.16397990166183754</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4949,11 +4267,11 @@
       </c>
       <c r="D87">
         <f t="shared" si="7"/>
-        <v>7.3038191067359017</v>
+        <v>2.362525274943799</v>
       </c>
       <c r="E87">
         <f t="shared" si="5"/>
-        <v>0.3631067036818893</v>
+        <v>0.15333697545768391</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4970,11 +4288,11 @@
       </c>
       <c r="D88">
         <f t="shared" si="7"/>
-        <v>6.9407124030540128</v>
+        <v>2.2091882994861152</v>
       </c>
       <c r="E88">
         <f t="shared" si="5"/>
-        <v>0.34505498630883269</v>
+        <v>0.14338481609165568</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4991,11 +4309,11 @@
       </c>
       <c r="D89">
         <f t="shared" si="7"/>
-        <v>6.5956574167451798</v>
+        <v>2.0658034833944594</v>
       </c>
       <c r="E89">
         <f t="shared" si="5"/>
-        <v>0.32790070348273559</v>
+        <v>0.13407859013960793</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -5012,11 +4330,11 @@
       </c>
       <c r="D90">
         <f t="shared" si="7"/>
-        <v>6.2677567132624441</v>
+        <v>1.9317248932548514</v>
       </c>
       <c r="E90">
         <f t="shared" si="5"/>
-        <v>0.3115992395723296</v>
+        <v>0.12537637403903013</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -5033,11 +4351,11 @@
       </c>
       <c r="D91">
         <f t="shared" si="7"/>
-        <v>5.9561574736901148</v>
+        <v>1.8063485192158213</v>
       </c>
       <c r="E91">
         <f t="shared" si="5"/>
-        <v>0.29610819699618673</v>
+        <v>0.11723896522783614</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -5054,11 +4372,11 @@
       </c>
       <c r="D92">
         <f t="shared" si="7"/>
-        <v>5.6600492766939281</v>
+        <v>1.6891095539879852</v>
       </c>
       <c r="E92">
         <f t="shared" si="5"/>
-        <v>0.28138728595317991</v>
+        <v>0.10962970554097307</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -5075,11 +4393,11 @@
       </c>
       <c r="D93">
         <f t="shared" si="7"/>
-        <v>5.3786619907407482</v>
+        <v>1.5794798484470123</v>
       </c>
       <c r="E93">
         <f t="shared" si="5"/>
-        <v>0.26739821963495419</v>
+        <v>0.10251431606926924</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -5096,11 +4414,11 @@
       </c>
       <c r="D94">
         <f t="shared" si="7"/>
-        <v>5.1112637711057944</v>
+        <v>1.4769655323777431</v>
       </c>
       <c r="E94">
         <f t="shared" si="5"/>
-        <v>0.25410461464787154</v>
+        <v>9.5860742736578131E-2</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -5117,11 +4435,11 @@
       </c>
       <c r="D95">
         <f t="shared" si="7"/>
-        <v>4.8571591564579233</v>
+        <v>1.381104789641165</v>
       </c>
       <c r="E95">
         <f t="shared" si="5"/>
-        <v>0.24147189638544192</v>
+        <v>8.963901189955939E-2</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -5138,11 +4456,11 @@
       </c>
       <c r="D96">
         <f t="shared" si="7"/>
-        <v>4.6156872600724812</v>
+        <v>1.2914657777416056</v>
       </c>
       <c r="E96">
         <f t="shared" si="5"/>
-        <v>0.22946720910512988</v>
+        <v>8.3821095319589367E-2</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -5159,11 +4477,11 @@
       </c>
       <c r="D97">
         <f t="shared" si="7"/>
-        <v>4.386220050967351</v>
+        <v>1.2076446824220164</v>
       </c>
       <c r="E97">
         <f t="shared" si="5"/>
-        <v>0.21805933047565995</v>
+        <v>7.8380783898513967E-2</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -5180,11 +4498,11 @@
       </c>
       <c r="D98">
         <f t="shared" si="7"/>
-        <v>4.1681607204916915</v>
+        <v>1.1292638985235024</v>
       </c>
       <c r="E98">
         <f t="shared" si="5"/>
-        <v>0.20721859037257137</v>
+        <v>7.3293569609436629E-2</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -5201,11 +4519,11 @@
       </c>
       <c r="D99">
         <f t="shared" si="7"/>
-        <v>3.9609421301191201</v>
+        <v>1.0559703289140658</v>
       </c>
       <c r="E99">
         <f t="shared" si="5"/>
-        <v>0.19691679371082216</v>
+        <v>6.8536535090652245E-2</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -5222,11 +4540,11 @@
       </c>
       <c r="D100">
         <f t="shared" si="7"/>
-        <v>3.7640253364082978</v>
+        <v>0.98743379382341356</v>
       </c>
       <c r="E100">
         <f t="shared" si="5"/>
-        <v>0.18712714711374237</v>
+        <v>6.4088250405359287E-2</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -5243,11 +4561,11 @@
       </c>
       <c r="D101">
         <f t="shared" si="7"/>
-        <v>3.5768981892945555</v>
+        <v>0.9233455434180543</v>
       </c>
       <c r="E101">
         <f t="shared" si="5"/>
-        <v>0.17782418922761359</v>
+        <v>5.9928676502063689E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>